<commit_message>
update(sanPham): validate các thuộc tính
</commit_message>
<xml_diff>
--- a/WebsiteTechWorldBackEnd/src/main/resources/templates/ModelSanPhamTemplate.xlsx
+++ b/WebsiteTechWorldBackEnd/src/main/resources/templates/ModelSanPhamTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACF04B8-7C7D-4499-B759-22239101921A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5C1633-B23A-447A-8999-40E36C0EE3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{6B43DE9F-2356-4B88-AF05-34F8AFB2CCE1}"/>
   </bookViews>
@@ -128,18 +128,9 @@
     <t>loaiCameraSau</t>
   </si>
   <si>
-    <t>Plus</t>
-  </si>
-  <si>
-    <t>doPhanGiaCameraSau</t>
-  </si>
-  <si>
     <t>khauDoCameraSau</t>
   </si>
   <si>
-    <t>iPhone 30Cường</t>
-  </si>
-  <si>
     <t>Wide, Ultra Wide, Telephoto</t>
   </si>
   <si>
@@ -147,6 +138,15 @@
   </si>
   <si>
     <t>f/1.6, f/2.4, f/2.8</t>
+  </si>
+  <si>
+    <t>doPhanGiaiCameraSau</t>
+  </si>
+  <si>
+    <t>iPhone 30</t>
+  </si>
+  <si>
+    <t>Thường</t>
   </si>
 </sst>
 </file>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D82C0B6-B55B-40B7-8DCB-60B61C6A25FE}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -629,15 +629,15 @@
         <v>29</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="S1" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B2" s="3">
         <v>45901</v>
@@ -682,16 +682,16 @@
         <v>27</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="S2" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>